<commit_message>
MOV SUB AND OR are done
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A284B2-D011-4293-9149-C2C51098A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE73EC-C67F-4965-9EAF-45BA3C9A0C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="111">
   <si>
     <t>op</t>
   </si>
@@ -507,10 +507,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2404,10 +2404,10 @@
       <c r="AE28">
         <v>0</v>
       </c>
-      <c r="AG28" s="16" t="s">
+      <c r="AG28" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="AH28" s="16"/>
+      <c r="AH28" s="17"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -2483,8 +2483,8 @@
       <c r="AE29">
         <v>0</v>
       </c>
-      <c r="AG29" s="16"/>
-      <c r="AH29" s="16"/>
+      <c r="AG29" s="17"/>
+      <c r="AH29" s="17"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -2560,8 +2560,8 @@
       <c r="AE30">
         <v>0</v>
       </c>
-      <c r="AG30" s="16"/>
-      <c r="AH30" s="16"/>
+      <c r="AG30" s="17"/>
+      <c r="AH30" s="17"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -2637,8 +2637,8 @@
       <c r="AE31">
         <v>0</v>
       </c>
-      <c r="AG31" s="16"/>
-      <c r="AH31" s="16"/>
+      <c r="AG31" s="17"/>
+      <c r="AH31" s="17"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
@@ -2906,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BEB407-C58A-4A68-8120-2B54FA5CBB73}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3054,7 +3054,7 @@
       <c r="F6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>67</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -3193,7 +3193,9 @@
       <c r="F12" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="H12" s="14" t="s">
         <v>101</v>
       </c>
@@ -3217,7 +3219,7 @@
       <c r="F13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>68</v>
       </c>
       <c r="H13" t="s">
@@ -3243,7 +3245,9 @@
       <c r="F14" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="H14" t="s">
         <v>103</v>
       </c>
@@ -3267,7 +3271,9 @@
       <c r="F15" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="H15" t="s">
         <v>104</v>
       </c>
@@ -3291,7 +3297,9 @@
       <c r="F16" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="17"/>
+      <c r="G16" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="H16" t="s">
         <v>105</v>
       </c>
@@ -3315,7 +3323,7 @@
       <c r="F17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="17"/>
+      <c r="G17" s="16"/>
       <c r="H17" t="s">
         <v>106</v>
       </c>
@@ -3339,7 +3347,7 @@
       <c r="F18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="16"/>
       <c r="H18" t="s">
         <v>107</v>
       </c>
@@ -3356,7 +3364,7 @@
         <v>85</v>
       </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
@@ -3377,7 +3385,7 @@
       <c r="F20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="15" t="s">
         <v>108</v>
       </c>
@@ -3401,7 +3409,7 @@
       <c r="F21" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="15" t="s">
         <v>108</v>
       </c>
@@ -3418,7 +3426,7 @@
         <v>85</v>
       </c>
       <c r="F22" s="10"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
@@ -3432,7 +3440,7 @@
         <v>85</v>
       </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
@@ -3453,7 +3461,7 @@
       <c r="F24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="16" t="s">
         <v>69</v>
       </c>
       <c r="H24" s="14" t="s">
@@ -3479,7 +3487,7 @@
       <c r="F25" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="16" t="s">
         <v>69</v>
       </c>
       <c r="H25" s="14" t="s">
@@ -3505,7 +3513,7 @@
       <c r="F26" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="16" t="s">
         <v>69</v>
       </c>
       <c r="H26" s="14" t="s">

</xml_diff>

<commit_message>
SETC CLCC are Done :D
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE73EC-C67F-4965-9EAF-45BA3C9A0C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D444D3C5-8B86-44F8-BFDB-A996F3BBF697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="110">
   <si>
     <t>op</t>
   </si>
@@ -367,9 +367,6 @@
   </si>
   <si>
     <t>3:0</t>
-  </si>
-  <si>
-    <t>?:</t>
   </si>
 </sst>
 </file>
@@ -2904,10 +2901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BEB407-C58A-4A68-8120-2B54FA5CBB73}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2921,7 +2918,7 @@
     <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>86</v>
       </c>
@@ -2941,7 +2938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>91</v>
       </c>
@@ -2961,7 +2958,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2987,7 +2984,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -3006,12 +3003,14 @@
       <c r="F4" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -3030,12 +3029,14 @@
       <c r="F5" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -3080,15 +3081,14 @@
       <c r="F7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="H7" t="s">
         <v>99</v>
       </c>
-      <c r="K7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -3107,12 +3107,14 @@
       <c r="F8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="H8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
@@ -3136,7 +3138,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
@@ -3160,7 +3162,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="C11" t="s">
         <v>85</v>
@@ -3172,9 +3174,8 @@
         <v>85</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -3200,7 +3201,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -3251,8 +3252,11 @@
       <c r="H14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -3323,7 +3327,9 @@
       <c r="F17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="H17" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
SHL SHR are done :D
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D444D3C5-8B86-44F8-BFDB-A996F3BBF697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49BF2FE-5C8B-4EA1-9F76-F93512874030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="120">
   <si>
     <t>op</t>
   </si>
@@ -367,6 +367,36 @@
   </si>
   <si>
     <t>3:0</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>xxxx</t>
   </si>
 </sst>
 </file>
@@ -821,148 +851,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143EB804-9F5F-4231-9BD8-F64F4BEDFFE9}">
-  <dimension ref="A1:AL37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D61745-689A-4B64-A3F1-FFF3B01003C8}">
+  <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.08984375" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" hidden="1" customWidth="1"/>
-    <col min="4" max="10" width="16.90625" hidden="1" customWidth="1"/>
-    <col min="11" max="17" width="8.7265625" customWidth="1"/>
-    <col min="22" max="26" width="8.7265625" customWidth="1"/>
-    <col min="30" max="30" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="7" width="16.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="14" width="8.81640625" customWidth="1"/>
+    <col min="15" max="15" width="8.90625" customWidth="1"/>
+    <col min="20" max="24" width="8.81640625" customWidth="1"/>
+    <col min="28" max="28" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" t="s">
-        <v>90</v>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
         <v>4</v>
       </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
       <c r="R1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="U1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="X1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="Y1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE1" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AF1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="B2" s="12">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C2" s="12">
         <v>0.6333333333333333</v>
       </c>
-      <c r="C2" s="12">
+      <c r="D2" s="12">
         <v>0.46458333333333335</v>
       </c>
-      <c r="D2" s="12">
+      <c r="E2" s="12">
         <v>0.33749999999999997</v>
       </c>
-      <c r="E2" s="12">
-        <v>0.16874999999999998</v>
-      </c>
       <c r="F2" s="12">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3">
+        <v>85</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
@@ -980,59 +1019,61 @@
       <c r="V3">
         <v>0</v>
       </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
+      <c r="AF3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>1</v>
       </c>
       <c r="AH3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AJ3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4">
+        <v>85</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1046,44 +1087,46 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>85</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5">
+        <v>85</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1097,47 +1140,49 @@
       <c r="V5">
         <v>0</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
+      <c r="AE5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
       </c>
       <c r="R6">
         <v>1</v>
@@ -1146,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1154,62 +1199,64 @@
       <c r="V6">
         <v>0</v>
       </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
+      <c r="AE6">
         <v>3</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>55</v>
       </c>
       <c r="AH6" t="s">
         <v>55</v>
       </c>
       <c r="AI6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AJ6" t="s">
         <v>55</v>
       </c>
-      <c r="AK6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>85</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
       </c>
       <c r="R7">
         <v>1</v>
@@ -1218,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -1226,50 +1273,52 @@
       <c r="V7">
         <v>0</v>
       </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AE7" t="s">
         <v>57</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AF7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1278,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1286,47 +1335,49 @@
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" t="s">
         <v>85</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" t="s">
-        <v>8</v>
-      </c>
-      <c r="O9">
+        <v>85</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9">
         <v>2</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
       <c r="R9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -1341,50 +1392,52 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9">
-        <v>1</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" t="s">
         <v>85</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" t="s">
-        <v>8</v>
-      </c>
-      <c r="O10">
+        <v>85</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
         <v>2</v>
       </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
       <c r="R10">
         <v>1</v>
       </c>
@@ -1392,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1404,67 +1457,62 @@
         <v>0</v>
       </c>
       <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C11" s="10"/>
+      <c r="D11" t="s">
         <v>85</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" t="s">
         <v>85</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
       <c r="K12" t="s">
         <v>8</v>
       </c>
-      <c r="L12" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12">
+      <c r="M12">
         <v>3</v>
       </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
       <c r="R12">
         <v>1</v>
       </c>
@@ -1472,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -1480,48 +1528,47 @@
       <c r="V12">
         <v>0</v>
       </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>85</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
       <c r="K13" t="s">
         <v>8</v>
       </c>
-      <c r="L13" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O13">
+      <c r="M13">
         <v>3</v>
       </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
       <c r="R13">
         <v>1</v>
       </c>
@@ -1529,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1537,48 +1584,47 @@
       <c r="V13">
         <v>0</v>
       </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" t="s">
         <v>85</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
       <c r="K14" t="s">
         <v>8</v>
       </c>
-      <c r="L14" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" t="s">
-        <v>8</v>
-      </c>
-      <c r="O14">
+      <c r="M14">
         <v>3</v>
       </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
       <c r="R14">
         <v>1</v>
       </c>
@@ -1586,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -1594,48 +1640,47 @@
       <c r="V14">
         <v>0</v>
       </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" t="s">
         <v>85</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
       <c r="K15" t="s">
         <v>8</v>
       </c>
-      <c r="L15" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" t="s">
-        <v>8</v>
-      </c>
-      <c r="O15">
+      <c r="M15">
         <v>3</v>
       </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
       <c r="R15">
         <v>1</v>
       </c>
@@ -1643,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -1651,48 +1696,47 @@
       <c r="V15">
         <v>0</v>
       </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" t="s">
         <v>85</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
       <c r="K16" t="s">
         <v>8</v>
       </c>
-      <c r="L16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M16" t="s">
-        <v>8</v>
-      </c>
-      <c r="O16">
+      <c r="M16">
         <v>3</v>
       </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
       <c r="R16">
         <v>1</v>
       </c>
@@ -1700,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -1708,56 +1752,55 @@
       <c r="V16">
         <v>0</v>
       </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" t="s">
         <v>85</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
         <v>8</v>
       </c>
       <c r="L17" t="s">
         <v>8</v>
       </c>
-      <c r="N17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O17">
+      <c r="M17">
         <v>4</v>
       </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
       <c r="R17">
         <v>1</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -1765,56 +1808,55 @@
       <c r="V17">
         <v>0</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
         <v>8</v>
       </c>
       <c r="L18" t="s">
         <v>8</v>
       </c>
-      <c r="N18" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18">
+      <c r="M18">
         <v>4</v>
       </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -1822,79 +1864,74 @@
       <c r="V18">
         <v>0</v>
       </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B19" s="10"/>
-      <c r="C19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="10" t="s">
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="C19" s="10"/>
+      <c r="D19" t="s">
         <v>85</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" t="s">
         <v>85</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
       <c r="K20" t="s">
         <v>8</v>
       </c>
-      <c r="M20" t="s">
-        <v>8</v>
-      </c>
-      <c r="O20">
+      <c r="M20">
         <v>5</v>
       </c>
-      <c r="P20" t="s">
+      <c r="N20" t="s">
         <v>50</v>
       </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
       <c r="R20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
         <v>0</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -1903,70 +1940,69 @@
         <v>0</v>
       </c>
       <c r="Y20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20">
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20">
         <v>0</v>
       </c>
-      <c r="AD20">
-        <v>1</v>
-      </c>
-      <c r="AE20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" t="s">
-        <v>8</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
         <v>49</v>
       </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
       <c r="R21">
         <v>1</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21">
         <v>1</v>
@@ -1975,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21">
         <v>0</v>
@@ -1990,134 +2026,125 @@
         <v>0</v>
       </c>
       <c r="AB21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21">
         <v>0</v>
       </c>
-      <c r="AD21">
-        <v>1</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
-      <c r="AG21" t="s">
+      <c r="AE21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B22" s="10"/>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="10" t="s">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="C22" s="10"/>
+      <c r="D22" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="P22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>46</v>
+      </c>
       <c r="R22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="U22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W22" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="X22" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="Y22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC22" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B23" s="10"/>
-      <c r="C23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="10" t="s">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="C23" s="10"/>
+      <c r="D23" t="s">
         <v>85</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" t="s">
         <v>85</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
       </c>
       <c r="R24">
         <v>1</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -2146,56 +2173,55 @@
       <c r="AC24">
         <v>0</v>
       </c>
-      <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
         <v>85</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
       <c r="K25" t="s">
         <v>8</v>
       </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O25">
+      <c r="M25">
         <v>6</v>
       </c>
-      <c r="R25" s="13">
+      <c r="P25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
         <v>1</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25">
         <v>1</v>
@@ -2204,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="W25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25">
         <v>0</v>
@@ -2224,62 +2250,61 @@
       <c r="AC25">
         <v>0</v>
       </c>
-      <c r="AD25">
-        <v>0</v>
-      </c>
-      <c r="AE25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="s">
         <v>85</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
       <c r="K26" t="s">
         <v>8</v>
       </c>
-      <c r="L26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>8</v>
-      </c>
-      <c r="O26">
+      <c r="M26">
         <v>7</v>
       </c>
-      <c r="R26" s="13">
-        <v>1</v>
+      <c r="P26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
       </c>
       <c r="S26">
         <v>0</v>
       </c>
       <c r="T26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26">
         <v>0</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -2302,64 +2327,59 @@
       <c r="AC26">
         <v>0</v>
       </c>
-      <c r="AD26">
-        <v>0</v>
-      </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B27" s="10"/>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="10" t="s">
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="C27" s="10"/>
+      <c r="D27" t="s">
         <v>85</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" t="s">
         <v>85</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" t="s">
-        <v>8</v>
-      </c>
-      <c r="L28" t="s">
-        <v>8</v>
-      </c>
-      <c r="O28">
-        <v>8</v>
-      </c>
-      <c r="R28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>8</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>51</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>51</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
       </c>
       <c r="S28" t="s">
         <v>51</v>
@@ -2371,19 +2391,19 @@
         <v>51</v>
       </c>
       <c r="V28">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
       </c>
       <c r="X28">
-        <v>1</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="Y28">
         <v>0</v>
       </c>
       <c r="Z28">
-        <f>0</f>
         <v>0</v>
       </c>
       <c r="AA28">
@@ -2395,51 +2415,50 @@
       <c r="AC28">
         <v>0</v>
       </c>
-      <c r="AD28">
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <v>0</v>
-      </c>
-      <c r="AG28" s="17" t="s">
+      <c r="AE28" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="AH28" s="17"/>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AF28" s="17"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" t="s">
-        <v>8</v>
-      </c>
-      <c r="L29" t="s">
-        <v>8</v>
-      </c>
-      <c r="O29">
-        <v>8</v>
-      </c>
-      <c r="R29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>8</v>
+      </c>
+      <c r="P29" t="s">
         <v>51</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>51</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
       </c>
       <c r="S29" t="s">
         <v>51</v>
@@ -2451,13 +2470,13 @@
         <v>51</v>
       </c>
       <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
       </c>
       <c r="X29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y29">
         <v>0</v>
@@ -2474,49 +2493,48 @@
       <c r="AC29">
         <v>0</v>
       </c>
-      <c r="AD29">
-        <v>0</v>
-      </c>
-      <c r="AE29">
-        <v>0</v>
-      </c>
-      <c r="AG29" s="17"/>
-      <c r="AH29" s="17"/>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="17"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" t="s">
         <v>85</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" t="s">
-        <v>8</v>
-      </c>
-      <c r="L30" t="s">
-        <v>8</v>
-      </c>
-      <c r="O30">
-        <v>8</v>
-      </c>
-      <c r="R30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30">
+        <v>8</v>
+      </c>
+      <c r="P30" t="s">
         <v>51</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
       </c>
       <c r="S30" t="s">
         <v>51</v>
@@ -2528,13 +2546,13 @@
         <v>51</v>
       </c>
       <c r="V30">
-        <v>0</v>
-      </c>
-      <c r="W30" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
       </c>
       <c r="X30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y30">
         <v>0</v>
@@ -2551,49 +2569,48 @@
       <c r="AC30">
         <v>0</v>
       </c>
-      <c r="AD30">
-        <v>0</v>
-      </c>
-      <c r="AE30">
-        <v>0</v>
-      </c>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="17"/>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE30" s="17"/>
+      <c r="AF30" s="17"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" t="s">
-        <v>8</v>
-      </c>
-      <c r="L31" t="s">
-        <v>8</v>
-      </c>
-      <c r="O31">
+        <v>85</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31">
         <v>9</v>
       </c>
-      <c r="R31" t="s">
+      <c r="P31" t="s">
         <v>51</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>51</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
       </c>
       <c r="S31" t="s">
         <v>51</v>
@@ -2605,13 +2622,13 @@
         <v>51</v>
       </c>
       <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
       </c>
       <c r="X31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y31">
         <v>0</v>
@@ -2628,55 +2645,51 @@
       <c r="AC31">
         <v>0</v>
       </c>
-      <c r="AD31">
-        <v>0</v>
-      </c>
-      <c r="AE31">
-        <v>0</v>
-      </c>
-      <c r="AG31" s="17"/>
-      <c r="AH31" s="17"/>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C32" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" t="s">
         <v>85</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" t="s">
-        <v>8</v>
-      </c>
-      <c r="L32" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" t="s">
+        <v>34</v>
       </c>
       <c r="P32" t="s">
-        <v>34</v>
-      </c>
-      <c r="R32" t="s">
         <v>51</v>
       </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
       <c r="S32">
         <v>0</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -2688,16 +2701,16 @@
         <v>0</v>
       </c>
       <c r="X32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB32">
         <v>1</v>
@@ -2705,53 +2718,49 @@
       <c r="AC32">
         <v>0</v>
       </c>
-      <c r="AD32">
-        <v>1</v>
-      </c>
-      <c r="AE32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" t="s">
+        <v>35</v>
       </c>
       <c r="P33" t="s">
-        <v>35</v>
-      </c>
-      <c r="R33" t="s">
         <v>51</v>
       </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
       <c r="S33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T33">
         <v>0</v>
       </c>
       <c r="U33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -2769,61 +2778,57 @@
         <v>0</v>
       </c>
       <c r="AA33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33">
         <v>1</v>
       </c>
-      <c r="AD33">
-        <v>1</v>
-      </c>
-      <c r="AE33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="C34" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
         <v>85</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" t="s">
+        <v>36</v>
       </c>
       <c r="P34" t="s">
-        <v>36</v>
-      </c>
-      <c r="R34" t="s">
         <v>51</v>
       </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
       <c r="S34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T34">
         <v>0</v>
       </c>
       <c r="U34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -2841,61 +2846,45 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34">
         <v>1</v>
       </c>
-      <c r="AD34">
-        <v>1</v>
-      </c>
-      <c r="AE34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36">
-        <v>1100</v>
-      </c>
-      <c r="K36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="K37" t="s">
-        <v>8</v>
+      <c r="I37" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
       </c>
       <c r="P37" t="s">
-        <v>37</v>
-      </c>
-      <c r="R37" t="s">
         <v>54</v>
       </c>
-      <c r="S37" t="s">
+      <c r="Q37" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AG28:AH31"/>
+    <mergeCell ref="AE28:AF31"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2903,8 +2892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BEB407-C58A-4A68-8120-2B54FA5CBB73}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2983,6 +2972,7 @@
       <c r="H3" s="15" t="s">
         <v>108</v>
       </c>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -3009,6 +2999,7 @@
       <c r="H4" s="10" t="s">
         <v>96</v>
       </c>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -3035,6 +3026,7 @@
       <c r="H5" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -3061,6 +3053,7 @@
       <c r="H6" s="10" t="s">
         <v>98</v>
       </c>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -3087,6 +3080,7 @@
       <c r="H7" t="s">
         <v>99</v>
       </c>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -3113,6 +3107,7 @@
       <c r="H8" t="s">
         <v>100</v>
       </c>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
@@ -3137,6 +3132,7 @@
       <c r="H9" s="15" t="s">
         <v>108</v>
       </c>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -3161,6 +3157,7 @@
       <c r="H10" s="15" t="s">
         <v>108</v>
       </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
@@ -3174,6 +3171,7 @@
         <v>85</v>
       </c>
       <c r="F11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -3200,6 +3198,7 @@
       <c r="H12" s="14" t="s">
         <v>101</v>
       </c>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -3226,6 +3225,7 @@
       <c r="H13" t="s">
         <v>102</v>
       </c>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -3252,6 +3252,7 @@
       <c r="H14" t="s">
         <v>103</v>
       </c>
+      <c r="I14" s="10"/>
       <c r="L14">
         <v>1001</v>
       </c>
@@ -3281,6 +3282,7 @@
       <c r="H15" t="s">
         <v>104</v>
       </c>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -3307,8 +3309,9 @@
       <c r="H16" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -3328,13 +3331,14 @@
         <v>76</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="H17" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -3353,12 +3357,15 @@
       <c r="F18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>111</v>
+      </c>
       <c r="H18" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
       <c r="C19" t="s">
         <v>85</v>
@@ -3371,8 +3378,9 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -3395,8 +3403,9 @@
       <c r="H20" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -3419,8 +3428,9 @@
       <c r="H21" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" s="10"/>
       <c r="C22" t="s">
         <v>85</v>
@@ -3433,8 +3443,9 @@
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
       <c r="C23" t="s">
         <v>85</v>
@@ -3447,8 +3458,9 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -3473,13 +3485,14 @@
       <c r="H24" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
         <v>85</v>
@@ -3499,13 +3512,14 @@
       <c r="H25" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>85</v>
@@ -3525,8 +3539,9 @@
       <c r="H26" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
       <c r="C27" t="s">
         <v>85</v>
@@ -3539,8 +3554,9 @@
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3563,8 +3579,9 @@
       <c r="H28" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -3587,8 +3604,9 @@
       <c r="H29" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -3611,8 +3629,9 @@
       <c r="H30" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -3635,8 +3654,9 @@
       <c r="H31" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
@@ -3656,8 +3676,9 @@
         <v>76</v>
       </c>
       <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -3677,13 +3698,14 @@
         <v>76</v>
       </c>
       <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
         <v>85</v>
@@ -3698,21 +3720,14 @@
         <v>78</v>
       </c>
       <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I34" s="10"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Updated Design with Push and Pop
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF6DB20-D9E1-4F04-85AF-228C6BD81437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA62868-BF17-46E6-8733-65C06F410BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="110">
   <si>
     <t>op</t>
   </si>
@@ -824,7 +824,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D61745-689A-4B64-A3F1-FFF3B01003C8}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2860,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BEB407-C58A-4A68-8120-2B54FA5CBB73}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3246,7 +3248,9 @@
       <c r="D20" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="F20" s="15" t="s">
         <v>98</v>
       </c>
@@ -3505,5 +3509,8 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Bugs of push and Pop Merge with Jump
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E4041D-9DC1-4755-9DA8-24536CFA73D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5C833-1A63-4D6E-A820-665DAF8137D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="110">
   <si>
     <t>op</t>
   </si>
@@ -2864,7 +2863,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3274,7 +3273,9 @@
       <c r="D21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="F21" s="15" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Added Test Case 15 TA
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Alu Operations.xlsx
+++ b/Phase2/Documentations/Alu Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5C833-1A63-4D6E-A820-665DAF8137D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3E0864-C7B7-448D-B784-2C1F9378858B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{A4E0179B-17F8-48EF-80B0-A3E450BF09FB}"/>
   </bookViews>
@@ -2863,7 +2863,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>